<commit_message>
Se modifco la base de datos
</commit_message>
<xml_diff>
--- a/QA-Tests/Sprint-2/Primera iteración - v1.3.0/Sprint 2 - CP primera iteración.xlsx
+++ b/QA-Tests/Sprint-2/Primera iteración - v1.3.0/Sprint 2 - CP primera iteración.xlsx
@@ -688,8 +688,8 @@
   </sheetPr>
   <dimension ref="B1:J1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>